<commit_message>
add GAN cifar10 yuv model
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="convnet" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="49">
   <si>
     <t xml:space="preserve">#</t>
   </si>
@@ -284,23 +284,23 @@
   <dimension ref="A1:O16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H17" activeCellId="0" sqref="H17"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13:O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.8724489795918"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="41.5765306122449"/>
-    <col collapsed="false" hidden="false" max="1023" min="16" style="1" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="1" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="12" min="10" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="41.0357142857143"/>
+    <col collapsed="false" hidden="false" max="1023" min="16" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1024" style="0" width="8.23469387755102"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -775,21 +775,28 @@
         <v>42</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0"/>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
-      <c r="D13" s="0"/>
-      <c r="E13" s="0"/>
-      <c r="F13" s="0"/>
-      <c r="G13" s="0"/>
-      <c r="H13" s="0"/>
-      <c r="I13" s="0"/>
-      <c r="J13" s="0"/>
-      <c r="K13" s="0"/>
-      <c r="L13" s="0"/>
-      <c r="M13" s="0"/>
-      <c r="N13" s="0"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <v>0.002</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>26</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="14.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0"/>
@@ -902,12 +909,12 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="H13:O13 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="8.10204081632653"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>